<commit_message>
création du projet vue
</commit_message>
<xml_diff>
--- a/FrontEnd/Sofiene/doc/Journal-de-Travail_BelkhiriaSofiene.xlsx
+++ b/FrontEnd/Sofiene/doc/Journal-de-Travail_BelkhiriaSofiene.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po66qga\Documents\GitHub\P_WEB295\FrontEnd\Sofiene\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{568286C2-94D3-48A2-A0F6-03E2431EE696}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3368944-AA59-48DD-8330-B03AF2A31994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7020" yWindow="3885" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -95,13 +95,13 @@
     <t>P_DB_I165</t>
   </si>
   <si>
-    <t>Répartition des tache</t>
-  </si>
-  <si>
     <t>Belkhiria Sofièene</t>
   </si>
   <si>
     <t>Mise en place des dossiers du projet</t>
+  </si>
+  <si>
+    <t>création du projet vue</t>
   </si>
 </sst>
 </file>
@@ -240,50 +240,6 @@
   </cellStyles>
   <dxfs count="13">
     <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -332,6 +288,50 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -346,7 +346,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{45CB4986-052B-374B-A8D0-88D41B362A09}" name="Table2" displayName="Table2" ref="A5:F507" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{45CB4986-052B-374B-A8D0-88D41B362A09}" name="Table2" displayName="Table2" ref="A5:F507" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="A5:F507" xr:uid="{45CB4986-052B-374B-A8D0-88D41B362A09}">
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -354,14 +354,14 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{F92771A6-FBDD-734E-AD68-EEBCABBE5406}" name="Semaine" dataDxfId="10">
+    <tableColumn id="1" xr3:uid="{F92771A6-FBDD-734E-AD68-EEBCABBE5406}" name="Semaine" dataDxfId="5">
       <calculatedColumnFormula>IF(ISBLANK(B6),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{8A6A2217-ACA1-B64A-AACC-E62161ECEC47}" name="Jour" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{7CF180A9-4021-614A-ABFA-FD02FA7EE89D}" name="Temps [h]" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{DA59D006-464D-084D-8523-AF3DB167EDE2}" name="Type" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{5207D366-301C-BA4D-A840-0D62AE8890E1}" name="Description" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{F7678D64-0216-D64A-A954-D1A966D4BF65}" name="Remarques/problèmes" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{8A6A2217-ACA1-B64A-AACC-E62161ECEC47}" name="Jour" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{7CF180A9-4021-614A-ABFA-FD02FA7EE89D}" name="Temps [h]" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{DA59D006-464D-084D-8523-AF3DB167EDE2}" name="Type" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{5207D366-301C-BA4D-A840-0D62AE8890E1}" name="Description" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{F7678D64-0216-D64A-A954-D1A966D4BF65}" name="Remarques/problèmes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -557,7 +557,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
+      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -591,7 +591,7 @@
         <v>16</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="5" t="s">
@@ -622,7 +622,7 @@
       </c>
       <c r="C3" s="22">
         <f>SUM(C5:C497)</f>
-        <v>9.7222222222222224E-3</v>
+        <v>1.3194444444444443E-2</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>13</v>
@@ -668,7 +668,7 @@
         <v>7</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F6" s="11"/>
     </row>
@@ -680,13 +680,13 @@
         <v>45405</v>
       </c>
       <c r="C7" s="23">
-        <v>2.7777777777777779E-3</v>
+        <v>6.2499999999999995E-3</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F7" s="11"/>
     </row>
@@ -6193,19 +6193,19 @@
   </sheetData>
   <sheetProtection insertHyperlinks="0" selectLockedCells="1" sort="0" autoFilter="0"/>
   <conditionalFormatting sqref="D6:D507">
-    <cfRule type="expression" dxfId="4" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="1" stopIfTrue="1">
       <formula>$D6="Meeting"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="11" priority="2">
       <formula>$D6="Documentation"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="3" stopIfTrue="1">
       <formula>$D6="Test"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="4" stopIfTrue="1">
       <formula>$D6="Analyse"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="6" stopIfTrue="1">
       <formula>$D6="Dévelopement"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6223,6 +6223,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="83ae57d85107fc73e8c281aedb059e49">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b000e6a26fbebedf4c24f086a5622afe" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -6445,27 +6465,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EB0028C-89CE-4553-AB94-94DC6E832369}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDECA689-F55E-43C8-8CEF-25DE741768EA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{146BE2DA-6117-4657-9EA0-437EBB1E64B8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6482,23 +6501,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDECA689-F55E-43C8-8CEF-25DE741768EA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EB0028C-89CE-4553-AB94-94DC6E832369}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
detail livre + suppréssion livre oke
</commit_message>
<xml_diff>
--- a/FrontEnd/Sofiene/doc/Journal-de-Travail_BelkhiriaSofiene.xlsx
+++ b/FrontEnd/Sofiene/doc/Journal-de-Travail_BelkhiriaSofiene.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po66qga\Documents\GitHub\P_WEB295\FrontEnd\Sofiene\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2CB5EA3-097E-4FDF-AAFD-68670099A83B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFDAC0C1-DA99-47BE-9C8F-63EE482741B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -108,6 +108,24 @@
   </si>
   <si>
     <t xml:space="preserve">Mise en place de la creation du compte </t>
+  </si>
+  <si>
+    <t>Page de connexion</t>
+  </si>
+  <si>
+    <t>Page d'ajout de livre</t>
+  </si>
+  <si>
+    <t>Le prof nous a parler du test</t>
+  </si>
+  <si>
+    <t>Revue du CDC avec Lucas</t>
+  </si>
+  <si>
+    <t>Mise en place de la page de détail du livre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mise en place du boutton permettant de supprimer les livres </t>
   </si>
 </sst>
 </file>
@@ -563,7 +581,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
+      <selection pane="bottomLeft" activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -628,7 +646,7 @@
       </c>
       <c r="C3" s="22">
         <f>SUM(C5:C497)</f>
-        <v>0.25528935185185186</v>
+        <v>0.48515046296296299</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>13</v>
@@ -733,69 +751,117 @@
       <c r="F9" s="11"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="str">
+      <c r="A10" s="15">
         <f>IF(ISBLANK(B10),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
+        <v>19</v>
+      </c>
+      <c r="B10" s="9">
+        <v>45418</v>
+      </c>
+      <c r="C10" s="10">
+        <v>5.347222222222222E-2</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>23</v>
+      </c>
       <c r="F10" s="11"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="str">
+      <c r="A11" s="15">
         <f>IF(ISBLANK(B11),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
+        <v>19</v>
+      </c>
+      <c r="B11" s="9">
+        <v>45418</v>
+      </c>
+      <c r="C11" s="10">
+        <v>7.1527777777777787E-2</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>24</v>
+      </c>
       <c r="F11" s="11"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="str">
+      <c r="A12" s="15">
         <f>IF(ISBLANK(B12),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
+        <v>20</v>
+      </c>
+      <c r="B12" s="9">
+        <v>45425</v>
+      </c>
+      <c r="C12" s="10">
+        <v>1.5972222222222224E-2</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>25</v>
+      </c>
       <c r="F12" s="11"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="15" t="str">
+      <c r="A13" s="15">
         <f>IF(ISBLANK(B13),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
+        <v>20</v>
+      </c>
+      <c r="B13" s="9">
+        <v>45425</v>
+      </c>
+      <c r="C13" s="10">
+        <v>9.0277777777777787E-3</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>26</v>
+      </c>
       <c r="F13" s="11"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="str">
+      <c r="A14" s="15">
         <f>IF(ISBLANK(B14),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B14" s="9"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
+        <v>20</v>
+      </c>
+      <c r="B14" s="9">
+        <v>45425</v>
+      </c>
+      <c r="C14" s="10">
+        <v>6.1111111111111116E-2</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>27</v>
+      </c>
       <c r="F14" s="11"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="15" t="str">
+      <c r="A15" s="15">
         <f>IF(ISBLANK(B15),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
+        <v>20</v>
+      </c>
+      <c r="B15" s="9">
+        <v>45425</v>
+      </c>
+      <c r="C15" s="10">
+        <v>1.8749999999999999E-2</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>28</v>
+      </c>
       <c r="F15" s="11"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -6243,26 +6309,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="83ae57d85107fc73e8c281aedb059e49">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b000e6a26fbebedf4c24f086a5622afe" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -6485,26 +6531,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EB0028C-89CE-4553-AB94-94DC6E832369}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDECA689-F55E-43C8-8CEF-25DE741768EA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{146BE2DA-6117-4657-9EA0-437EBB1E64B8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6521,4 +6568,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDECA689-F55E-43C8-8CEF-25DE741768EA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EB0028C-89CE-4553-AB94-94DC6E832369}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>